<commit_message>
working with demo sit
</commit_message>
<xml_diff>
--- a/target/test-classes/dataEngine/DataEngine.xlsx
+++ b/target/test-classes/dataEngine/DataEngine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -284,13 +284,17 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,13 +718,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.7109375" style="4" collapsed="1"/>
-    <col min="3" max="3" width="51.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.7109375" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" style="4" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="51.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="24.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="4" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -965,7 +969,9 @@
       <c r="F12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G12"/>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1170,10 +1176,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="8.7109375" style="10" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="10" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="10" width="41.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="10" width="12.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="10" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1214,7 +1220,9 @@
       <c r="C3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">

</xml_diff>